<commit_message>
[FIX] Add counselor for student at import process
</commit_message>
<xml_diff>
--- a/public/templates/Template Siswa.xlsx
+++ b/public/templates/Template Siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\appiks-be\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{488B646C-C7ED-4BC0-B281-6B9DF7208F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284ED2E8-4FB2-401B-BDB3-A7B80B841B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C10B551-A4DA-49C4-BF89-947AAA021A36}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NIS</t>
   </si>
@@ -44,10 +44,13 @@
     <t>Nama</t>
   </si>
   <si>
-    <t>NIP</t>
+    <t>Kode Kelas</t>
   </si>
   <si>
-    <t>Kode Kelas</t>
+    <t>NIP Wali</t>
+  </si>
+  <si>
+    <t>NIP BK</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C57A01B-1527-4F3F-AC07-15D83CC5F91B}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,7 +434,7 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,10 +442,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Column text format for excel template
</commit_message>
<xml_diff>
--- a/public/templates/Template Siswa.xlsx
+++ b/public/templates/Template Siswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\appiks-be\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284ED2E8-4FB2-401B-BDB3-A7B80B841B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2C085-B111-49B5-9119-DF313D4704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C10B551-A4DA-49C4-BF89-947AAA021A36}"/>
   </bookViews>
@@ -86,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,29 +426,31 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] Use NISN for student import and handle schedule job
</commit_message>
<xml_diff>
--- a/public/templates/Template Siswa.xlsx
+++ b/public/templates/Template Siswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\appiks-be\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2C085-B111-49B5-9119-DF313D4704D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492092C7-BCDA-4BFC-BD88-EF83D60A06C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C10B551-A4DA-49C4-BF89-947AAA021A36}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>NIS</t>
-  </si>
-  <si>
     <t>Nama</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>NIP BK</t>
+  </si>
+  <si>
+    <t>NISN</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,19 +439,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>